<commit_message>
modificado json ciudad y vehiculos
</commit_message>
<xml_diff>
--- a/tests/Prueba_exploratoria.xlsx
+++ b/tests/Prueba_exploratoria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="9240" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
   <si>
     <t>#</t>
   </si>
@@ -132,9 +132,6 @@
     <t>EL HEADER INCLUYE A IZQUIERDA LOGO Y LEMA CLICKEABLES</t>
   </si>
   <si>
-    <t>pendiente, se ve mal el texto de la card</t>
-  </si>
-  <si>
     <t>no hay pagina, se usó Modal</t>
   </si>
   <si>
@@ -156,19 +153,19 @@
     <t>x</t>
   </si>
   <si>
-    <t>No se pudo probar por falla de logueo</t>
-  </si>
-  <si>
     <t>Boton dice "ver más"</t>
   </si>
   <si>
     <t>Se usa Modal. De fondo el Header y el Buscador</t>
   </si>
   <si>
-    <t>pendiente ver botones en categoria</t>
-  </si>
-  <si>
     <t>no hay pagina, se usó Modal. De fondo se ve.</t>
+  </si>
+  <si>
+    <t>Por ahora hay una sóla Pagina</t>
+  </si>
+  <si>
+    <t>pendiente, ver texto de card y header</t>
   </si>
 </sst>
 </file>
@@ -687,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,7 +726,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -737,16 +734,14 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>2</v>
-      </c>
+      <c r="E4" s="13"/>
       <c r="F4" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>47</v>
@@ -757,17 +752,17 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -775,7 +770,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>8</v>
@@ -799,7 +794,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -815,7 +810,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -823,7 +818,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>8</v>
@@ -839,17 +834,17 @@
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -857,17 +852,17 @@
         <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -875,10 +870,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>2</v>
@@ -891,25 +886,23 @@
         <v>10</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="E13" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>13</v>
@@ -925,7 +918,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>14</v>
@@ -951,7 +944,7 @@
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -969,7 +962,7 @@
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -977,7 +970,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>16</v>
@@ -993,7 +986,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>15</v>
@@ -1009,7 +1002,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>17</v>
@@ -1025,7 +1018,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>18</v>
@@ -1041,7 +1034,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>19</v>
@@ -1057,7 +1050,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>20</v>
@@ -1073,7 +1066,7 @@
         <v>21</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>21</v>
@@ -1089,7 +1082,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>22</v>
@@ -1105,7 +1098,7 @@
         <v>23</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>23</v>
@@ -1121,7 +1114,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>24</v>
@@ -1131,7 +1124,7 @@
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1149,7 +1142,7 @@
       </c>
       <c r="F28" s="13"/>
       <c r="G28" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -1167,7 +1160,7 @@
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1185,7 +1178,7 @@
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1203,7 +1196,7 @@
       </c>
       <c r="F31" s="13"/>
       <c r="G31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1216,20 +1209,18 @@
       <c r="D32" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="E32" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" s="13"/>
+      <c r="G32" s="2"/>
     </row>
     <row r="33" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>30</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>32</v>
@@ -1239,7 +1230,7 @@
       </c>
       <c r="F33" s="13"/>
       <c r="G33" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -1247,7 +1238,7 @@
         <v>31</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>33</v>
@@ -1257,7 +1248,7 @@
       </c>
       <c r="F34" s="13"/>
       <c r="G34" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1265,18 +1256,16 @@
         <v>32</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>44</v>
-      </c>
+      <c r="E35" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="14"/>
+      <c r="G35" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="E3:F35"/>

</xml_diff>

<commit_message>
mejoro tablas testeosv2 y exploratoria en dev
</commit_message>
<xml_diff>
--- a/tests/Prueba_exploratoria.xlsx
+++ b/tests/Prueba_exploratoria.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="5280" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Exploratorio Sprint 2 " sheetId="2" r:id="rId1"/>
+    <sheet name="Exploratorio Sprint 1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$E$3:$F$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Exploratorio Sprint 1'!$E$3:$F$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Exploratorio Sprint 2 '!$F$3:$G$39</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="74">
   <si>
     <t>#</t>
   </si>
@@ -132,6 +134,9 @@
     <t>EL HEADER INCLUYE A IZQUIERDA LOGO Y LEMA CLICKEABLES</t>
   </si>
   <si>
+    <t>pendiente, se ve mal el texto de la card</t>
+  </si>
+  <si>
     <t>no hay pagina, se usó Modal</t>
   </si>
   <si>
@@ -153,19 +158,94 @@
     <t>x</t>
   </si>
   <si>
+    <t>No se pudo probar por falla de logueo</t>
+  </si>
+  <si>
     <t>Boton dice "ver más"</t>
   </si>
   <si>
     <t>Se usa Modal. De fondo el Header y el Buscador</t>
   </si>
   <si>
+    <t>pendiente ver botones en categoria</t>
+  </si>
+  <si>
     <t>no hay pagina, se usó Modal. De fondo se ve.</t>
   </si>
   <si>
-    <t>Por ahora hay una sóla Pagina</t>
-  </si>
-  <si>
-    <t>pendiente, ver texto de card y header</t>
+    <t>comentarios spring1</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>PAGINA PRODUCTO</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>AL SELECCIONAR UN VEHICULO E INGRESAR A LA PAGINA SE OBTIENE UNA URL AMIGABLE</t>
+  </si>
+  <si>
+    <t>DESDE LA PAGINA DE PRODUCTO PUEDO SALIR ( FLECHA ATRÁS) HACIA LA HOME.</t>
+  </si>
+  <si>
+    <t>CONTIENE LOS SIGUIENTES BLOQUES: HEADER, UBICACIÓN, IMÁGENES, DESCRIPCION, CARACTERISTICAS, POLITICAS, RESERVAS</t>
+  </si>
+  <si>
+    <t>EL BLOQUE HEADER CONTIENE LA CATEGORIA DEL PRODUCTO, EL TITULO Y UNA FLECHA BACK</t>
+  </si>
+  <si>
+    <t>EL BLOQUE UBICACION CONTIENE LA UBICACIÓN DEL PRODUCTO</t>
+  </si>
+  <si>
+    <t>EN FORMATO DESKTOP EL BLOQUE IMÁGENES CONTIENE  5 IMÁGENES UNA GRANDE Y OTRAS 4 MAS CHICAS EN GRILLA DE 2 X2 , CON BORDES REDONDEADOS Y UN BOTON QUE DICE "VER MAS" PARA ACCEDER A MAS FOTOS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EN FORMATO TABLET EL BLOQUE IMÁGENES CONTIENE  1 IMAGEN  QUE CUBRE EL 100% DEL ANCHO Y LA IMAGEN CAMBIAS CADA 3 SEGUNDOS. DEBAJO UN INDICADOR CON EL NUMERO DE FOTO ACTUAL Y EL TOTAL DE IMAGENES. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EN FORMATO PHONE EL BLOQUE IMÁGENES CONTIENE  1 IMAGEN  QUE CUBRE EL 100% DEL ANCHO Y LA IMAGEN CAMBIAS CADA 3 SEGUNDOS. DEBAJO UN INDICADOR CON EL NUMERO DE FOTO ACTUAL Y EL TOTAL DE IMAGENES. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EN FORMATO DESKTOP, EL BLOQUE CARACTERISTICAS CONTIENE EL TITULO Y UNA GRILLA DE 4 COLUMNAS CON ATRIBUTOS ASOCIADOS A SU ICONO CORRESPONDIENTE.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EN FORMATO TABLET, EL BLOQUE CARACTERISTICAS CONTIENE EL TITULO Y UNA GRILLA DE 2 COLUMNAS CON ATRIBUTOS ASOCIADOS A SU ICONO CORRESPONDIENTE.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EN FORMATO PHONE, EL BLOQUE CARACTERISTICAS CONTIENE EL TITULO Y UNA GRILLA DE 1 COLUMNA CON ATRIBUTOS ASOCIADOS A SU ICONO CORRESPONDIENTE.  </t>
+  </si>
+  <si>
+    <t>EL BLOQUE DESCRIPCION CONTIENE EL TITULO Y UN TEXTO DE DESCRIPCION. ES RESPONSIVE A TABLET Y PHONE</t>
+  </si>
+  <si>
+    <t>EN FORMATO DESKTOP, EL BLOQUE POLITICAS  CONTIENE EL TITULO Y UNA GRILLA DE 3 COLUMNAS Y EN CADA UNA UN TITULO Y UNA DESCRPICON.</t>
+  </si>
+  <si>
+    <t>EN FORMATO TABLET, EL BLOQUE POLITICAS  CONTIENE EL TITULO Y UNA GRILLA DE 2 COLUMNAS Y EN CADA UNA UN TITULO Y UNA DESCRPICON.</t>
+  </si>
+  <si>
+    <t>EN FORMATO PHONE, EL BLOQUE POLITICAS  CONTIENE EL TITULO Y UNA GRILLA DE 1 COLUMNA Y EN CADA UNA UN TITULO Y UNA DESCRPICON.</t>
+  </si>
+  <si>
+    <t>EN FORMATO DESKTOP, EL BLOQUE RESERVAS CONTIENE UN CALENDARIO ALINEADO A IZQUIERDA QUE MUESTRE 2 MESES E INDICA TANTO LAS FECHAS DISPONIBLES COMO LAS NO DISPONIBLES. AL LADO UN BOTON DE INICIAR RESERVA.</t>
+  </si>
+  <si>
+    <t>EN FORMATO TABLET, EL BLOQUE RESERVAS CONTIENE UN CALENDARIO ALINEADO A IZQUIERDA QUE MUESTRE 2 MESES E INDCA TANTO LAS FECHAS DISPONIBLES COMO LAS NO DISPONIBLES. DEBAJO UN BOTON DE INICIAR RESERVA.</t>
+  </si>
+  <si>
+    <t>EN FORMATO TABLET, EL BLOQUE RESERVAS CONTIENE UN CALENDARIO ALINEADO A IZQUIERDA QUE MUESTRE 1 MES E INDCA TANTO LAS FECHAS DISPONIBLES COMO LAS NO DISPONIBLES. DEBAJO UN BOTON DE INICIAR RESERVA.</t>
+  </si>
+  <si>
+    <t>AL INICIAR LA PAGINA ME MUESTRA UN GRUPO RANDOM DE VEHICULOS, REINICIANDO SE MODIFICAN</t>
+  </si>
+  <si>
+    <t>SELECCIONANDO UNA CIUDAD Y PRESIONANDO BUSCAR NO RENDERIZA LSO PRODUCTOS DIPONIBLES EN ESA CIUDAD</t>
+  </si>
+  <si>
+    <t>CREADO</t>
   </si>
 </sst>
 </file>
@@ -195,7 +275,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -334,11 +414,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -384,6 +538,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -401,6 +558,38 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -682,10 +871,1151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="54.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="45.5703125" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="32"/>
+      <c r="H2" s="33"/>
+    </row>
+    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="21"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>33</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="25"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="3">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="3">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>35</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="25"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="3">
+        <v>6</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="3">
+        <v>7</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="3">
+        <v>8</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>9</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="2:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>10</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="3">
+        <v>11</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>12</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <v>13</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="3">
+        <v>14</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>15</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>16</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>17</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="3">
+        <v>18</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>19</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="3">
+        <v>20</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
+        <v>21</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="2:9" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
+        <v>22</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>23</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="3">
+        <v>24</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>25</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
+        <v>26</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <v>27</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
+        <v>28</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" s="13"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
+        <v>29</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
+        <v>30</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" s="13"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="4">
+        <v>31</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="4">
+        <v>32</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H39" s="2"/>
+      <c r="I39" s="27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="4">
+        <v>36</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="4">
+        <v>37</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B42" s="4">
+        <v>38</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="4">
+        <v>39</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="4">
+        <v>40</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B45" s="4">
+        <v>41</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B46" s="4">
+        <v>42</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="2:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B47" s="4">
+        <v>43</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="4">
+        <v>44</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B49" s="4">
+        <v>45</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B50" s="4">
+        <v>46</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B51" s="4">
+        <v>47</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B52" s="4">
+        <v>48</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B53" s="4">
+        <v>49</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B54" s="4">
+        <v>50</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="B55" s="4">
+        <v>51</v>
+      </c>
+      <c r="C55" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B56" s="4">
+        <v>52</v>
+      </c>
+      <c r="C56" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B57" s="4">
+        <v>53</v>
+      </c>
+      <c r="C57" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B58" s="4">
+        <v>54</v>
+      </c>
+      <c r="C58" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="2:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="29">
+        <v>55</v>
+      </c>
+      <c r="C59" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="30"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="F3:G39"/>
+  <mergeCells count="4">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,25 +2030,25 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="20"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="11" t="s">
         <v>2</v>
       </c>
@@ -726,7 +2056,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
@@ -734,14 +2064,16 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="13" t="s">
+        <v>2</v>
+      </c>
       <c r="F4" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>47</v>
@@ -752,17 +2084,17 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -770,7 +2102,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>8</v>
@@ -794,7 +2126,7 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
@@ -810,7 +2142,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -818,7 +2150,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>8</v>
@@ -834,17 +2166,17 @@
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -852,17 +2184,17 @@
         <v>8</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -870,10 +2202,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>2</v>
@@ -886,23 +2218,25 @@
         <v>10</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="2"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>11</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>13</v>
@@ -918,7 +2252,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>14</v>
@@ -944,7 +2278,7 @@
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -962,7 +2296,7 @@
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -970,7 +2304,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>16</v>
@@ -986,7 +2320,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>15</v>
@@ -1002,7 +2336,7 @@
         <v>17</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>17</v>
@@ -1018,7 +2352,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>18</v>
@@ -1034,7 +2368,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>19</v>
@@ -1050,7 +2384,7 @@
         <v>20</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>20</v>
@@ -1066,7 +2400,7 @@
         <v>21</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>21</v>
@@ -1082,7 +2416,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>22</v>
@@ -1098,7 +2432,7 @@
         <v>23</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>23</v>
@@ -1114,7 +2448,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>24</v>
@@ -1124,7 +2458,7 @@
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1142,7 +2476,7 @@
       </c>
       <c r="F28" s="13"/>
       <c r="G28" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -1160,7 +2494,7 @@
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1178,7 +2512,7 @@
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -1196,7 +2530,7 @@
       </c>
       <c r="F31" s="13"/>
       <c r="G31" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="45" x14ac:dyDescent="0.25">
@@ -1209,18 +2543,20 @@
       <c r="D32" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="2"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="33" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="3">
         <v>30</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>32</v>
@@ -1230,7 +2566,7 @@
       </c>
       <c r="F33" s="13"/>
       <c r="G33" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -1238,7 +2574,7 @@
         <v>31</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>33</v>
@@ -1248,7 +2584,7 @@
       </c>
       <c r="F34" s="13"/>
       <c r="G34" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1256,16 +2592,18 @@
         <v>32</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="E35" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="16"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="E3:F35"/>

</xml_diff>

<commit_message>
mas avances en testeos
</commit_message>
<xml_diff>
--- a/tests/Prueba_exploratoria.xlsx
+++ b/tests/Prueba_exploratoria.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="15840" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="818"/>
   </bookViews>
   <sheets>
     <sheet name="Exploratorio Sprint 4" sheetId="4" r:id="rId1"/>
     <sheet name="Exploratorio Sprint 3" sheetId="3" r:id="rId2"/>
     <sheet name="Exploratorio Sprint 2 " sheetId="2" r:id="rId3"/>
     <sheet name="Exploratorio Sprint 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Resumen Errores" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Exploratorio Sprint 1'!$E$3:$F$35</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="144">
   <si>
     <t>#</t>
   </si>
@@ -394,6 +395,72 @@
   </si>
   <si>
     <t>AL NO PODER DAR DE ALTA UN PRODUCTO, APRECE UN CARTEL DE ALERTA</t>
+  </si>
+  <si>
+    <t>ESTADO ORIGEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRIORIDAD </t>
+  </si>
+  <si>
+    <t>SEVERIDAD</t>
+  </si>
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t>SPRING/ CICLO</t>
+  </si>
+  <si>
+    <t>ESTADO ACTUAL</t>
+  </si>
+  <si>
+    <t>COMENTARIO</t>
+  </si>
+  <si>
+    <t>´01</t>
+  </si>
+  <si>
+    <t>A RESOLVER</t>
+  </si>
+  <si>
+    <t>MEDIA</t>
+  </si>
+  <si>
+    <t>BAJA</t>
+  </si>
+  <si>
+    <t>RESUELTO</t>
+  </si>
+  <si>
+    <t>´02</t>
+  </si>
+  <si>
+    <t>ALTA</t>
+  </si>
+  <si>
+    <t>DEPRECATED</t>
+  </si>
+  <si>
+    <t>´07</t>
+  </si>
+  <si>
+    <t>´15</t>
+  </si>
+  <si>
+    <t>Prueba</t>
+  </si>
+  <si>
+    <t>VERIFICADO EN CICLO SPRING 2</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>VERIFICADO EN CICLO SPRING 3</t>
+  </si>
+  <si>
+    <t>AL DAR DE ALTA UN PRODUCTO, LAS FECHAS DE LA RESERVA A PARECEN BLOQUEADAS PARA UNA FUTURA RESERVA.</t>
   </si>
 </sst>
 </file>
@@ -653,7 +720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -738,6 +805,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -765,14 +841,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1327,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1382,29 +1461,29 @@
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="37" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="17"/>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41"/>
       <c r="I9" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="33"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="31" t="s">
         <v>71</v>
       </c>
@@ -1577,7 +1656,7 @@
       <c r="D18" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="32" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1585,13 +1664,13 @@
       <c r="B19" s="1">
         <v>70</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="E19" s="32" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1599,13 +1678,13 @@
       <c r="B20" s="1">
         <v>71</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="32" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1613,13 +1692,13 @@
       <c r="B21" s="1">
         <v>72</v>
       </c>
-      <c r="C21" s="42" t="s">
+      <c r="C21" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="D21" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="E21" s="41" t="s">
+      <c r="E21" s="32" t="s">
         <v>115</v>
       </c>
       <c r="I21" s="18"/>
@@ -1629,13 +1708,13 @@
       <c r="B22" s="1">
         <v>73</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="D22" s="43" t="s">
+      <c r="D22" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="E22" s="32" t="s">
         <v>115</v>
       </c>
       <c r="I22" s="18"/>
@@ -1645,20 +1724,31 @@
       <c r="B23" s="1">
         <v>74</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="43" t="s">
+      <c r="D23" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="E23" s="41" t="s">
+      <c r="E23" s="32" t="s">
         <v>115</v>
       </c>
       <c r="I23" s="18"/>
       <c r="J23" s="18"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C24" s="42"/>
+    <row r="24" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>75</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>115</v>
+      </c>
       <c r="I24" s="18"/>
       <c r="J24" s="18"/>
     </row>
@@ -1733,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,29 +1878,29 @@
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="37" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="17"/>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41"/>
       <c r="I9" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="33"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
       <c r="E10" s="28" t="s">
         <v>71</v>
       </c>
@@ -2358,8 +2448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J59"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2376,26 +2466,26 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="37" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="17"/>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="37"/>
-      <c r="H2" s="38"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="33"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="24" t="s">
         <v>71</v>
       </c>
@@ -3579,8 +3669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3595,25 +3685,25 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="43"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="33"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="11" t="s">
         <v>2</v>
       </c>
@@ -4181,4 +4271,506 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="44"/>
+    <col min="2" max="2" width="17.42578125" style="44" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="44" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="44" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="44" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="44" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="44" customWidth="1"/>
+    <col min="8" max="8" width="39.42578125" style="44" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="44"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="45">
+        <v>44860</v>
+      </c>
+      <c r="F3" s="44">
+        <v>1</v>
+      </c>
+      <c r="G3" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="45">
+        <v>44860</v>
+      </c>
+      <c r="F4" s="44">
+        <v>1</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="45">
+        <v>44860</v>
+      </c>
+      <c r="F5" s="44">
+        <v>1</v>
+      </c>
+      <c r="G5" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="45">
+        <v>44860</v>
+      </c>
+      <c r="F6" s="44">
+        <v>1</v>
+      </c>
+      <c r="G6" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="44">
+        <v>10</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="45">
+        <v>44860</v>
+      </c>
+      <c r="F7" s="44">
+        <v>1</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="44">
+        <v>29</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="45">
+        <v>44860</v>
+      </c>
+      <c r="F8" s="44">
+        <v>1</v>
+      </c>
+      <c r="G8" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="44">
+        <v>32</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="45">
+        <v>44860</v>
+      </c>
+      <c r="F9" s="44">
+        <v>1</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H9" s="44" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="44">
+        <v>18</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="45">
+        <v>44874</v>
+      </c>
+      <c r="F10" s="44">
+        <v>2</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="44">
+        <v>23</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="45">
+        <v>44874</v>
+      </c>
+      <c r="F11" s="44">
+        <v>2</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="44">
+        <v>34</v>
+      </c>
+      <c r="B12" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="45">
+        <v>44874</v>
+      </c>
+      <c r="F12" s="44">
+        <v>2</v>
+      </c>
+      <c r="G12" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="44">
+        <v>43</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="45">
+        <v>44874</v>
+      </c>
+      <c r="F13" s="44">
+        <v>2</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="44">
+        <v>51</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="45">
+        <v>44874</v>
+      </c>
+      <c r="F14" s="44">
+        <v>2</v>
+      </c>
+      <c r="G14" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="44">
+        <v>52</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="45">
+        <v>44874</v>
+      </c>
+      <c r="F15" s="44">
+        <v>2</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="44">
+        <v>53</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="45">
+        <v>44874</v>
+      </c>
+      <c r="F16" s="44">
+        <v>2</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" s="44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="47">
+        <v>58</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="45">
+        <v>44889</v>
+      </c>
+      <c r="F17" s="44">
+        <v>3</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="44">
+        <v>59</v>
+      </c>
+      <c r="B18" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="45">
+        <v>44889</v>
+      </c>
+      <c r="F18" s="44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="44">
+        <v>63</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="45">
+        <v>44889</v>
+      </c>
+      <c r="F19" s="44">
+        <v>3</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" s="45">
+        <v>44889</v>
+      </c>
+      <c r="F20" s="44">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Info final de testing
</commit_message>
<xml_diff>
--- a/tests/Prueba_exploratoria.xlsx
+++ b/tests/Prueba_exploratoria.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="15840" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="818"/>
+    <workbookView xWindow="17160" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="818" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Exploratorio Sprint 4" sheetId="4" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Exploratorio Sprint 1'!$E$3:$F$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Exploratorio Sprint 2 '!$F$3:$G$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Exploratorio Sprint 3'!$F$10:$G$14</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Exploratorio Sprint 4'!$F$10:$G$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Exploratorio Sprint 4'!$F$4:$G$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="153">
   <si>
     <t>#</t>
   </si>
@@ -445,9 +445,6 @@
     <t>´07</t>
   </si>
   <si>
-    <t>´15</t>
-  </si>
-  <si>
     <t>Prueba</t>
   </si>
   <si>
@@ -460,7 +457,37 @@
     <t>VERIFICADO EN CICLO SPRING 3</t>
   </si>
   <si>
-    <t>AL DAR DE ALTA UN PRODUCTO, LAS FECHAS DE LA RESERVA A PARECEN BLOQUEADAS PARA UNA FUTURA RESERVA.</t>
+    <t>VERIFICADO EN CICLO SPRING 4</t>
+  </si>
+  <si>
+    <t>DA UN CÓDIGO 200 . Deprecated</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> trae info, no figura ciudad. Deprecated</t>
+  </si>
+  <si>
+    <t>RESULTADO SPRINT 3</t>
+  </si>
+  <si>
+    <t>Mejorado</t>
+  </si>
+  <si>
+    <t>No puede forzarse el error desde el front.</t>
+  </si>
+  <si>
+    <t>Permite faltando modelo y descripcion</t>
+  </si>
+  <si>
+    <t>ALTA DE reserva</t>
+  </si>
+  <si>
+    <t>AL DAR DE ALTA UNA RESERVA, LAS FECHAS DE LA RESERVA A PARECEN BLOQUEADAS PARA UNA FUTURA RESERVA.</t>
+  </si>
+  <si>
+    <t>Creación Producto</t>
+  </si>
+  <si>
+    <t>VERIFICADO EN CICLO SPRING 4 bis</t>
   </si>
 </sst>
 </file>
@@ -503,7 +530,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -716,11 +743,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -802,17 +879,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -841,18 +930,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1404,10 +1507,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J40"/>
+  <dimension ref="B1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="54.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="38.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="44"/>
+      <c r="H3" s="45"/>
+      <c r="I3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="40"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="26"/>
+    </row>
+    <row r="5" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>18</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="18"/>
+    </row>
+    <row r="6" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>58</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J6" s="18"/>
+    </row>
+    <row r="7" spans="2:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>59</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="25"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>63</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>66</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="49" t="s">
+        <v>146</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="50">
+        <v>69</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="51" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="50">
+        <v>70</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="48"/>
+      <c r="H11" s="51"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="50">
+        <v>71</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="48"/>
+      <c r="H12" s="51"/>
+    </row>
+    <row r="13" spans="2:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="50">
+        <v>72</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="48"/>
+      <c r="G13" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>148</v>
+      </c>
+      <c r="I13" s="18"/>
+      <c r="J13" s="18"/>
+    </row>
+    <row r="14" spans="2:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="50">
+        <v>73</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" s="48"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="18"/>
+      <c r="J14" s="18"/>
+    </row>
+    <row r="15" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="50">
+        <v>74</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" s="48"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+    </row>
+    <row r="16" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="52">
+        <v>75</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="E16" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="56"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+    </row>
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+    </row>
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+    </row>
+    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+    </row>
+    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+    </row>
+    <row r="21" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I21" s="27"/>
+      <c r="J21" s="18"/>
+    </row>
+    <row r="22" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+    </row>
+    <row r="23" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J23" s="18"/>
+    </row>
+    <row r="24" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J24" s="18"/>
+    </row>
+    <row r="25" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J25" s="18"/>
+    </row>
+    <row r="26" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="18"/>
+    </row>
+    <row r="27" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J27" s="18"/>
+    </row>
+    <row r="28" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="18"/>
+    </row>
+    <row r="30" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J30" s="18"/>
+    </row>
+    <row r="31" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J31" s="18"/>
+    </row>
+    <row r="32" spans="9:10" x14ac:dyDescent="0.25">
+      <c r="J32" s="18"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="F4:G5"/>
+  <mergeCells count="4">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:J54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1461,446 +1945,29 @@
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="41" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="17"/>
-      <c r="F9" s="39" t="s">
+      <c r="F9" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="40"/>
-      <c r="H9" s="41"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="45"/>
       <c r="I9" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="36"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="H10" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="26"/>
-    </row>
-    <row r="11" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
-        <v>18</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" s="18"/>
-    </row>
-    <row r="12" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="4">
-        <v>58</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="J12" s="18"/>
-    </row>
-    <row r="13" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
-        <v>59</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="4">
-        <v>63</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
-        <v>66</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G15" s="13"/>
-      <c r="H15" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
-        <v>67</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="2:10" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="20">
-        <v>68</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="21"/>
-    </row>
-    <row r="18" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="1">
-        <v>69</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E18" s="32" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
-        <v>70</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="D19" s="34" t="s">
-        <v>117</v>
-      </c>
-      <c r="E19" s="32" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="1">
-        <v>71</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="34" t="s">
-        <v>118</v>
-      </c>
-      <c r="E20" s="32" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="1">
-        <v>72</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="D21" s="34" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-    </row>
-    <row r="22" spans="2:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="1">
-        <v>73</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="D22" s="34" t="s">
-        <v>120</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-    </row>
-    <row r="23" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="1">
-        <v>74</v>
-      </c>
-      <c r="C23" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-    </row>
-    <row r="24" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B24" s="1">
-        <v>75</v>
-      </c>
-      <c r="C24" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I29" s="27"/>
-      <c r="J29" s="18"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I30" s="18"/>
-      <c r="J30" s="18"/>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J31" s="18"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J32" s="18"/>
-    </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J33" s="18"/>
-    </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J34" s="18"/>
-    </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J35" s="18"/>
-    </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J36" s="18"/>
-    </row>
-    <row r="37" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J37" s="18"/>
-    </row>
-    <row r="38" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J38" s="18"/>
-    </row>
-    <row r="39" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J39" s="18"/>
-    </row>
-    <row r="40" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J40" s="18"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="F10:G11"/>
-  <mergeCells count="4">
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="F9:H9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J54"/>
-  <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="54.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="31.7109375" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="39" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" s="40"/>
-      <c r="H9" s="41"/>
-      <c r="I9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="36"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="28" t="s">
         <v>71</v>
       </c>
@@ -2448,8 +2515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J59"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2466,26 +2533,26 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="41" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="17"/>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="36"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="24" t="s">
         <v>71</v>
       </c>
@@ -3685,25 +3752,25 @@
   <sheetData>
     <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="43"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="47"/>
     </row>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="36"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="11" t="s">
         <v>2</v>
       </c>
@@ -4277,497 +4344,509 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="44"/>
-    <col min="2" max="2" width="17.42578125" style="44" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" style="44" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="44" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="44" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="44" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" style="44" customWidth="1"/>
-    <col min="8" max="8" width="39.42578125" style="44" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="44"/>
+    <col min="1" max="1" width="11.42578125" style="35"/>
+    <col min="2" max="2" width="17.42578125" style="35" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" style="35" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" style="35" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="35" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="35" customWidth="1"/>
+    <col min="7" max="7" width="26.140625" style="35" customWidth="1"/>
+    <col min="8" max="8" width="39.42578125" style="35" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="35"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="36">
+        <v>44860</v>
+      </c>
+      <c r="F3" s="35">
+        <v>1</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="36">
+        <v>44860</v>
+      </c>
+      <c r="F4" s="35">
+        <v>1</v>
+      </c>
+      <c r="G4" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="F2" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="G2" s="44" t="s">
-        <v>127</v>
-      </c>
-      <c r="H2" s="44" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="44" t="s">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="C5" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D5" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="36">
+        <v>44860</v>
+      </c>
+      <c r="F5" s="35">
+        <v>1</v>
+      </c>
+      <c r="G5" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="E3" s="45">
+      <c r="D6" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="36">
         <v>44860</v>
       </c>
-      <c r="F3" s="44">
+      <c r="F6" s="35">
         <v>1</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G6" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="H6" s="35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
+        <v>10</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="36">
+        <v>44860</v>
+      </c>
+      <c r="F7" s="35">
+        <v>1</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="35">
+        <v>29</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="E8" s="36">
+        <v>44860</v>
+      </c>
+      <c r="F8" s="35">
+        <v>1</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="35">
+        <v>32</v>
+      </c>
+      <c r="B9" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="36">
+        <v>44860</v>
+      </c>
+      <c r="F9" s="35">
+        <v>1</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="35">
+        <v>18</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="36">
+        <v>44874</v>
+      </c>
+      <c r="F10" s="35">
+        <v>2</v>
+      </c>
+      <c r="G10" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="35">
+        <v>23</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="36">
+        <v>44874</v>
+      </c>
+      <c r="F11" s="35">
+        <v>2</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="35">
+        <v>34</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="36">
+        <v>44874</v>
+      </c>
+      <c r="F12" s="35">
+        <v>2</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="35">
+        <v>43</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="E13" s="36">
+        <v>44874</v>
+      </c>
+      <c r="F13" s="35">
+        <v>2</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="35">
+        <v>51</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14" s="36">
+        <v>44874</v>
+      </c>
+      <c r="F14" s="35">
+        <v>2</v>
+      </c>
+      <c r="G14" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="35">
+        <v>52</v>
+      </c>
+      <c r="B15" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C15" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D15" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="E15" s="36">
+        <v>44874</v>
+      </c>
+      <c r="F15" s="35">
+        <v>2</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="35">
+        <v>53</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="36">
+        <v>44874</v>
+      </c>
+      <c r="F16" s="35">
+        <v>2</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="38">
+        <v>58</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="36">
+        <v>44889</v>
+      </c>
+      <c r="F17" s="35">
+        <v>3</v>
+      </c>
+      <c r="G17" s="35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="35">
+        <v>59</v>
+      </c>
+      <c r="B18" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="36">
+        <v>44889</v>
+      </c>
+      <c r="F18" s="35">
+        <v>3</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H18" s="35" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
-        <v>134</v>
-      </c>
-      <c r="B4" s="44" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="35">
+        <v>63</v>
+      </c>
+      <c r="B19" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C19" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>132</v>
+      </c>
+      <c r="E19" s="36">
+        <v>44889</v>
+      </c>
+      <c r="F19" s="35">
+        <v>3</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="35">
+        <v>72</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="45">
-        <v>44860</v>
-      </c>
-      <c r="F4" s="44">
-        <v>1</v>
-      </c>
-      <c r="G4" s="44" t="s">
+      <c r="D20" s="35" t="s">
+        <v>135</v>
+      </c>
+      <c r="E20" s="36">
+        <v>44905</v>
+      </c>
+      <c r="F20" s="35">
+        <v>4</v>
+      </c>
+      <c r="G20" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="H4" s="44" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="45">
-        <v>44860</v>
-      </c>
-      <c r="F5" s="44">
-        <v>1</v>
-      </c>
-      <c r="G5" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H5" s="44" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="B6" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="E6" s="45">
-        <v>44860</v>
-      </c>
-      <c r="F6" s="44">
-        <v>1</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H6" s="44" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="44">
-        <v>10</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D7" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="E7" s="45">
-        <v>44860</v>
-      </c>
-      <c r="F7" s="44">
-        <v>1</v>
-      </c>
-      <c r="G7" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H7" s="44" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="44">
-        <v>29</v>
-      </c>
-      <c r="B8" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="E8" s="45">
-        <v>44860</v>
-      </c>
-      <c r="F8" s="44">
-        <v>1</v>
-      </c>
-      <c r="G8" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H8" s="44" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="44">
-        <v>32</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D9" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="E9" s="45">
-        <v>44860</v>
-      </c>
-      <c r="F9" s="44">
-        <v>1</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H9" s="44" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="44">
-        <v>18</v>
-      </c>
-      <c r="B10" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" s="45">
-        <v>44874</v>
-      </c>
-      <c r="F10" s="44">
-        <v>2</v>
-      </c>
-      <c r="G10" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H10" s="44" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="44">
-        <v>23</v>
-      </c>
-      <c r="B11" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="E11" s="45">
-        <v>44874</v>
-      </c>
-      <c r="F11" s="44">
-        <v>2</v>
-      </c>
-      <c r="G11" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H11" s="44" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="44">
-        <v>34</v>
-      </c>
-      <c r="B12" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" s="45">
-        <v>44874</v>
-      </c>
-      <c r="F12" s="44">
-        <v>2</v>
-      </c>
-      <c r="G12" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H12" s="44" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="44">
-        <v>43</v>
-      </c>
-      <c r="B13" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D13" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="E13" s="45">
-        <v>44874</v>
-      </c>
-      <c r="F13" s="44">
-        <v>2</v>
-      </c>
-      <c r="G13" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H13" s="44" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="44">
-        <v>51</v>
-      </c>
-      <c r="B14" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D14" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14" s="45">
-        <v>44874</v>
-      </c>
-      <c r="F14" s="44">
-        <v>2</v>
-      </c>
-      <c r="G14" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H14" s="44" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="44">
-        <v>52</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D15" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="45">
-        <v>44874</v>
-      </c>
-      <c r="F15" s="44">
-        <v>2</v>
-      </c>
-      <c r="G15" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H15" s="44" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="44">
-        <v>53</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C16" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="45">
-        <v>44874</v>
-      </c>
-      <c r="F16" s="44">
-        <v>2</v>
-      </c>
-      <c r="G16" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="H16" s="44" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="47">
-        <v>58</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C17" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="D17" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="E17" s="45">
-        <v>44889</v>
-      </c>
-      <c r="F17" s="44">
-        <v>3</v>
-      </c>
-      <c r="G17" s="44" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44">
-        <v>59</v>
-      </c>
-      <c r="B18" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C18" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D18" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="E18" s="45">
-        <v>44889</v>
-      </c>
-      <c r="F18" s="44">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="44">
-        <v>63</v>
-      </c>
-      <c r="B19" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C19" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="D19" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="E19" s="45">
-        <v>44889</v>
-      </c>
-      <c r="F19" s="44">
-        <v>3</v>
-      </c>
-      <c r="G19" s="44" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="C20" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D20" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="E20" s="45">
-        <v>44889</v>
-      </c>
-      <c r="F20" s="44">
-        <v>3</v>
+      <c r="H20" s="35" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>